<commit_message>
Cap nhat lại Phieu van dap.xlsx
</commit_message>
<xml_diff>
--- a/+ Ban nop/Phieu van dap.xlsx
+++ b/+ Ban nop/Phieu van dap.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="PhieuVanDap" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -421,7 +421,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -430,37 +430,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
@@ -473,30 +449,55 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -794,7 +795,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -808,107 +811,117 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="E2" s="30"/>
+      <c r="E2" s="25"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="32"/>
+      <c r="C3" s="33">
+        <v>0.9</v>
+      </c>
+      <c r="D3" s="27"/>
+      <c r="E3" s="28"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="32"/>
+      <c r="C4" s="33">
+        <v>0.89</v>
+      </c>
+      <c r="D4" s="27"/>
+      <c r="E4" s="28"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="32"/>
+      <c r="C5" s="33">
+        <v>0.97</v>
+      </c>
+      <c r="D5" s="27"/>
+      <c r="E5" s="28"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="32"/>
+      <c r="C6" s="33">
+        <v>0.97</v>
+      </c>
+      <c r="D6" s="27"/>
+      <c r="E6" s="28"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="32"/>
+      <c r="C7" s="33">
+        <v>0.99</v>
+      </c>
+      <c r="D7" s="27"/>
+      <c r="E7" s="28"/>
     </row>
     <row r="9" spans="1:8" ht="31.5">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
     </row>
     <row r="11" spans="1:8" ht="45">
       <c r="A11" s="2" t="s">
@@ -940,13 +953,13 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
       <c r="F12">
         <f>SUM(C13:C26)</f>
         <v>3.25</v>
@@ -957,163 +970,163 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="5">
+      <c r="A13" s="20">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="20">
         <v>0.75</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="21">
         <v>0.75</v>
       </c>
-      <c r="E13" s="8"/>
+      <c r="E13" s="23"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="5"/>
-      <c r="B14" s="9" t="s">
+      <c r="A14" s="20"/>
+      <c r="B14" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="5"/>
-      <c r="B15" s="9" t="s">
+      <c r="A15" s="20"/>
+      <c r="B15" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6" t="s">
+      <c r="A16" s="20"/>
+      <c r="B16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="5">
+      <c r="A17" s="20">
         <v>1.2</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="20">
         <v>1</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="21">
         <v>1</v>
       </c>
-      <c r="E17" s="8"/>
+      <c r="E17" s="23"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="5"/>
-      <c r="B18" s="9" t="s">
+      <c r="A18" s="20"/>
+      <c r="B18" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="5"/>
-      <c r="B19" s="9" t="s">
+      <c r="A19" s="20"/>
+      <c r="B19" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="5"/>
-      <c r="B20" s="9" t="s">
+      <c r="A20" s="20"/>
+      <c r="B20" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="5"/>
-      <c r="B21" s="9" t="s">
+      <c r="A21" s="20"/>
+      <c r="B21" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="5"/>
-      <c r="B22" s="9" t="s">
+      <c r="A22" s="20"/>
+      <c r="B22" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="5">
+      <c r="A23" s="20">
         <v>1.3</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="20">
         <v>1</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="21">
         <v>0.75</v>
       </c>
-      <c r="E23" s="8"/>
+      <c r="E23" s="23"/>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="5"/>
-      <c r="B24" s="9" t="s">
+      <c r="A24" s="20"/>
+      <c r="B24" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="32"/>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="5"/>
-      <c r="B25" s="9" t="s">
+      <c r="A25" s="20"/>
+      <c r="B25" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="12">
+      <c r="A26" s="6">
         <v>1.4</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="12">
+      <c r="C26" s="6">
         <v>0.5</v>
       </c>
-      <c r="D26" s="14">
+      <c r="D26" s="8">
         <v>1</v>
       </c>
-      <c r="E26" s="12"/>
+      <c r="E26" s="6"/>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
       <c r="F27">
         <f>SUM(C28:C41)</f>
         <v>4</v>
@@ -1124,169 +1137,169 @@
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="5">
+      <c r="A28" s="20">
         <v>2.1</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="5">
+      <c r="C28" s="20">
         <v>0.75</v>
       </c>
-      <c r="D28" s="7">
+      <c r="D28" s="21">
         <v>1</v>
       </c>
-      <c r="E28" s="8"/>
+      <c r="E28" s="23"/>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="5"/>
-      <c r="B29" s="9" t="s">
+      <c r="A29" s="20"/>
+      <c r="B29" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="5"/>
-      <c r="B30" s="9" t="s">
+      <c r="A30" s="20"/>
+      <c r="B30" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="5"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="5"/>
-      <c r="B31" s="6" t="s">
+      <c r="A31" s="20"/>
+      <c r="B31" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="5">
+      <c r="A32" s="20">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C32" s="20">
         <v>0.5</v>
       </c>
-      <c r="D32" s="7">
+      <c r="D32" s="21">
         <v>1</v>
       </c>
-      <c r="E32" s="8"/>
+      <c r="E32" s="23"/>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="5"/>
-      <c r="B33" s="9" t="s">
+      <c r="A33" s="20"/>
+      <c r="B33" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="5"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="22"/>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="5">
+      <c r="A34" s="20">
         <v>2.2999999999999998</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="5">
+      <c r="C34" s="20">
         <v>0.75</v>
       </c>
-      <c r="D34" s="7">
+      <c r="D34" s="21">
         <v>1</v>
       </c>
-      <c r="E34" s="8"/>
+      <c r="E34" s="23"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="5"/>
-      <c r="B35" s="9" t="s">
+      <c r="A35" s="20"/>
+      <c r="B35" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="5"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="32"/>
+      <c r="E35" s="32"/>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="5"/>
-      <c r="B36" s="9" t="s">
+      <c r="A36" s="20"/>
+      <c r="B36" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="5"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="22"/>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="5">
+      <c r="A37" s="20">
         <v>2.4</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C37" s="5">
+      <c r="C37" s="20">
         <v>1.5</v>
       </c>
-      <c r="D37" s="7">
+      <c r="D37" s="21">
         <v>1</v>
       </c>
-      <c r="E37" s="8"/>
+      <c r="E37" s="23"/>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="5"/>
-      <c r="B38" s="9" t="s">
+      <c r="A38" s="20"/>
+      <c r="B38" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="5"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
+      <c r="C38" s="20"/>
+      <c r="D38" s="32"/>
+      <c r="E38" s="32"/>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="5"/>
-      <c r="B39" s="9" t="s">
+      <c r="A39" s="20"/>
+      <c r="B39" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C39" s="5"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="32"/>
+      <c r="E39" s="32"/>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="5"/>
-      <c r="B40" s="9" t="s">
+      <c r="A40" s="20"/>
+      <c r="B40" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C40" s="5"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="11"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="12">
+      <c r="A41" s="6">
         <v>2.5</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C41" s="12">
+      <c r="C41" s="6">
         <v>0.5</v>
       </c>
-      <c r="D41" s="14">
+      <c r="D41" s="8">
         <v>1</v>
       </c>
-      <c r="E41" s="12"/>
+      <c r="E41" s="6"/>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
+      <c r="B42" s="31"/>
+      <c r="C42" s="31"/>
+      <c r="D42" s="31"/>
+      <c r="E42" s="31"/>
       <c r="F42">
         <f>SUM(C43:C45)</f>
         <v>1.5</v>
@@ -1297,58 +1310,58 @@
       </c>
     </row>
     <row r="43" spans="1:7">
-      <c r="A43" s="12">
+      <c r="A43" s="6">
         <v>3.1</v>
       </c>
-      <c r="B43" s="13" t="s">
+      <c r="B43" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C43" s="12">
+      <c r="C43" s="6">
         <v>0.5</v>
       </c>
-      <c r="D43" s="14">
+      <c r="D43" s="8">
         <v>0</v>
       </c>
-      <c r="E43" s="12"/>
+      <c r="E43" s="6"/>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="12">
+      <c r="A44" s="6">
         <v>3.2</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B44" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C44" s="12">
+      <c r="C44" s="6">
         <v>0.5</v>
       </c>
-      <c r="D44" s="14">
+      <c r="D44" s="8">
         <v>0</v>
       </c>
-      <c r="E44" s="12"/>
+      <c r="E44" s="6"/>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="12">
+      <c r="A45" s="6">
         <v>3.3</v>
       </c>
-      <c r="B45" s="13" t="s">
+      <c r="B45" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C45" s="12">
+      <c r="C45" s="6">
         <v>0.5</v>
       </c>
-      <c r="D45" s="14">
+      <c r="D45" s="8">
         <v>0</v>
       </c>
-      <c r="E45" s="12"/>
+      <c r="E45" s="6"/>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="B46" s="4"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="4"/>
+      <c r="B46" s="31"/>
+      <c r="C46" s="31"/>
+      <c r="D46" s="31"/>
+      <c r="E46" s="31"/>
       <c r="F46">
         <f>SUM(C47:C55)</f>
         <v>2.75</v>
@@ -1359,152 +1372,121 @@
       </c>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="5">
+      <c r="A47" s="20">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="B47" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C47" s="5">
+      <c r="C47" s="20">
         <v>0.5</v>
       </c>
-      <c r="D47" s="7">
+      <c r="D47" s="21">
         <v>0.25</v>
       </c>
-      <c r="E47" s="8"/>
+      <c r="E47" s="23"/>
     </row>
     <row r="48" spans="1:7">
-      <c r="A48" s="5"/>
-      <c r="B48" s="9" t="s">
+      <c r="A48" s="20"/>
+      <c r="B48" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C48" s="5"/>
-      <c r="D48" s="10"/>
-      <c r="E48" s="10"/>
+      <c r="C48" s="20"/>
+      <c r="D48" s="32"/>
+      <c r="E48" s="32"/>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" s="5"/>
-      <c r="B49" s="9" t="s">
+      <c r="A49" s="20"/>
+      <c r="B49" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C49" s="5"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="11"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="22"/>
+      <c r="E49" s="22"/>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="5">
+      <c r="A50" s="20">
         <v>4.2</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="B50" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C50" s="5">
+      <c r="C50" s="20">
         <v>1</v>
       </c>
-      <c r="D50" s="15">
+      <c r="D50" s="29">
         <v>0</v>
       </c>
-      <c r="E50" s="8"/>
+      <c r="E50" s="23"/>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="5"/>
-      <c r="B51" s="9" t="s">
+      <c r="A51" s="20"/>
+      <c r="B51" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C51" s="5"/>
-      <c r="D51" s="16"/>
-      <c r="E51" s="11"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="30"/>
+      <c r="E51" s="22"/>
     </row>
     <row r="52" spans="1:6">
-      <c r="A52" s="5">
+      <c r="A52" s="20">
         <v>4.3</v>
       </c>
-      <c r="B52" s="6" t="s">
+      <c r="B52" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C52" s="5">
+      <c r="C52" s="20">
         <v>0.5</v>
       </c>
-      <c r="D52" s="15">
+      <c r="D52" s="29">
         <v>1</v>
       </c>
-      <c r="E52" s="8"/>
+      <c r="E52" s="23"/>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="5"/>
-      <c r="B53" s="9" t="s">
+      <c r="A53" s="20"/>
+      <c r="B53" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C53" s="5"/>
-      <c r="D53" s="16"/>
-      <c r="E53" s="11"/>
+      <c r="C53" s="20"/>
+      <c r="D53" s="30"/>
+      <c r="E53" s="22"/>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="5">
+      <c r="A54" s="20">
         <v>4.4000000000000004</v>
       </c>
-      <c r="B54" s="17" t="s">
+      <c r="B54" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C54" s="5">
+      <c r="C54" s="20">
         <v>0.75</v>
       </c>
-      <c r="D54" s="7">
+      <c r="D54" s="21">
         <v>1</v>
       </c>
-      <c r="E54" s="8"/>
+      <c r="E54" s="23"/>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="5"/>
-      <c r="B55" s="9" t="s">
+      <c r="A55" s="20"/>
+      <c r="B55" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C55" s="5"/>
-      <c r="D55" s="11"/>
-      <c r="E55" s="11"/>
+      <c r="C55" s="20"/>
+      <c r="D55" s="22"/>
+      <c r="E55" s="22"/>
     </row>
     <row r="57" spans="1:6">
-      <c r="F57" s="18"/>
+      <c r="F57" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="E50:E51"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="A42:E42"/>
-    <mergeCell ref="A46:E46"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="D47:D49"/>
-    <mergeCell ref="E47:E49"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="C34:C36"/>
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="E34:E36"/>
-    <mergeCell ref="A37:A40"/>
-    <mergeCell ref="C37:C40"/>
-    <mergeCell ref="D37:D40"/>
-    <mergeCell ref="E37:E40"/>
-    <mergeCell ref="A27:E27"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="C28:C31"/>
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="E28:E31"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="D13:D16"/>
+    <mergeCell ref="E13:E16"/>
     <mergeCell ref="A32:A33"/>
     <mergeCell ref="C32:C33"/>
     <mergeCell ref="D32:D33"/>
@@ -1517,12 +1499,43 @@
     <mergeCell ref="C23:C25"/>
     <mergeCell ref="D23:D25"/>
     <mergeCell ref="E23:E25"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="C13:C16"/>
-    <mergeCell ref="D13:D16"/>
-    <mergeCell ref="E13:E16"/>
-    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="A27:E27"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="E28:E31"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="D47:D49"/>
+    <mergeCell ref="E47:E49"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="E34:E36"/>
+    <mergeCell ref="A37:A40"/>
+    <mergeCell ref="C37:C40"/>
+    <mergeCell ref="D37:D40"/>
+    <mergeCell ref="E37:E40"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="E50:E51"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="A42:E42"/>
+    <mergeCell ref="A46:E46"/>
+    <mergeCell ref="A47:A49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Cập nhật Phieu van dap.xlsx
</commit_message>
<xml_diff>
--- a/+ Ban nop/Phieu van dap.xlsx
+++ b/+ Ban nop/Phieu van dap.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="PhieuVanDap" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -458,46 +458,46 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -795,9 +795,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -814,12 +812,12 @@
       <c r="A1" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="19" t="s">
@@ -831,10 +829,10 @@
       <c r="C2" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="E2" s="25"/>
+      <c r="E2" s="31"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="18" t="s">
@@ -843,11 +841,11 @@
       <c r="B3" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="33">
+      <c r="C3" s="20">
         <v>0.9</v>
       </c>
-      <c r="D3" s="27"/>
-      <c r="E3" s="28"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="22"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="18" t="s">
@@ -856,11 +854,11 @@
       <c r="B4" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="33">
+      <c r="C4" s="20">
         <v>0.89</v>
       </c>
-      <c r="D4" s="27"/>
-      <c r="E4" s="28"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="22"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="18" t="s">
@@ -869,11 +867,11 @@
       <c r="B5" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="33">
+      <c r="C5" s="20">
         <v>0.97</v>
       </c>
-      <c r="D5" s="27"/>
-      <c r="E5" s="28"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="22"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="18" t="s">
@@ -882,11 +880,11 @@
       <c r="B6" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="C6" s="33">
+      <c r="C6" s="20">
         <v>0.97</v>
       </c>
-      <c r="D6" s="27"/>
-      <c r="E6" s="28"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="22"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="18" t="s">
@@ -895,11 +893,11 @@
       <c r="B7" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="C7" s="33">
+      <c r="C7" s="20">
         <v>0.99</v>
       </c>
-      <c r="D7" s="27"/>
-      <c r="E7" s="28"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="22"/>
     </row>
     <row r="9" spans="1:8" ht="31.5">
       <c r="A9" s="11" t="s">
@@ -945,164 +943,164 @@
       </c>
       <c r="G11">
         <f>SUM(G12,G27,G42,G46)</f>
-        <v>8.1875</v>
+        <v>10</v>
       </c>
       <c r="H11">
         <f>G11*3.75/10</f>
-        <v>3.0703125</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="31"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
       <c r="F12">
         <f>SUM(C13:C26)</f>
         <v>3.25</v>
       </c>
       <c r="G12">
         <f>C13*D13+C17*D17+C23*D23+C26*D26</f>
-        <v>2.8125</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="20">
+      <c r="A13" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="20">
+      <c r="C13" s="24">
         <v>0.75</v>
       </c>
-      <c r="D13" s="21">
-        <v>0.75</v>
-      </c>
-      <c r="E13" s="23"/>
+      <c r="D13" s="25">
+        <v>1</v>
+      </c>
+      <c r="E13" s="28"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="20"/>
+      <c r="A14" s="24"/>
       <c r="B14" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="20"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="20"/>
+      <c r="A15" s="24"/>
       <c r="B15" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="20"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="20"/>
+      <c r="A16" s="24"/>
       <c r="B16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="20">
+      <c r="A17" s="24">
         <v>1.2</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="20">
-        <v>1</v>
-      </c>
-      <c r="D17" s="21">
-        <v>1</v>
-      </c>
-      <c r="E17" s="23"/>
+      <c r="C17" s="24">
+        <v>1</v>
+      </c>
+      <c r="D17" s="25">
+        <v>1</v>
+      </c>
+      <c r="E17" s="28"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="20"/>
+      <c r="A18" s="24"/>
       <c r="B18" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="20"/>
+      <c r="A19" s="24"/>
       <c r="B19" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="20"/>
+      <c r="A20" s="24"/>
       <c r="B20" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="20"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="20"/>
+      <c r="A21" s="24"/>
       <c r="B21" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="20"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="20"/>
+      <c r="A22" s="24"/>
       <c r="B22" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="20"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="20">
+      <c r="A23" s="24">
         <v>1.3</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="20">
-        <v>1</v>
-      </c>
-      <c r="D23" s="21">
+      <c r="C23" s="24">
+        <v>1</v>
+      </c>
+      <c r="D23" s="25">
         <v>0.75</v>
       </c>
-      <c r="E23" s="23"/>
+      <c r="E23" s="28"/>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="20"/>
+      <c r="A24" s="24"/>
       <c r="B24" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="20"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="32"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="20"/>
+      <c r="A25" s="24"/>
       <c r="B25" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="20"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="22"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="6">
@@ -1120,13 +1118,13 @@
       <c r="E26" s="6"/>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
       <c r="F27">
         <f>SUM(C28:C41)</f>
         <v>4</v>
@@ -1137,145 +1135,145 @@
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="20">
+      <c r="A28" s="24">
         <v>2.1</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="20">
+      <c r="C28" s="24">
         <v>0.75</v>
       </c>
-      <c r="D28" s="21">
-        <v>1</v>
-      </c>
-      <c r="E28" s="23"/>
+      <c r="D28" s="25">
+        <v>1</v>
+      </c>
+      <c r="E28" s="28"/>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="20"/>
+      <c r="A29" s="24"/>
       <c r="B29" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="20"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="32"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="20"/>
+      <c r="A30" s="24"/>
       <c r="B30" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="20"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="32"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="20"/>
+      <c r="A31" s="24"/>
       <c r="B31" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="20"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="20">
+      <c r="A32" s="24">
         <v>2.2000000000000002</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="20">
+      <c r="C32" s="24">
         <v>0.5</v>
       </c>
-      <c r="D32" s="21">
-        <v>1</v>
-      </c>
-      <c r="E32" s="23"/>
+      <c r="D32" s="25">
+        <v>1</v>
+      </c>
+      <c r="E32" s="28"/>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="20"/>
+      <c r="A33" s="24"/>
       <c r="B33" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="20"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="22"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="20">
+      <c r="A34" s="24">
         <v>2.2999999999999998</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="20">
+      <c r="C34" s="24">
         <v>0.75</v>
       </c>
-      <c r="D34" s="21">
-        <v>1</v>
-      </c>
-      <c r="E34" s="23"/>
+      <c r="D34" s="25">
+        <v>1</v>
+      </c>
+      <c r="E34" s="28"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="20"/>
+      <c r="A35" s="24"/>
       <c r="B35" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="20"/>
-      <c r="D35" s="32"/>
-      <c r="E35" s="32"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="26"/>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="20"/>
+      <c r="A36" s="24"/>
       <c r="B36" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="20"/>
-      <c r="D36" s="22"/>
-      <c r="E36" s="22"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="27"/>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="20">
+      <c r="A37" s="24">
         <v>2.4</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C37" s="20">
+      <c r="C37" s="24">
         <v>1.5</v>
       </c>
-      <c r="D37" s="21">
-        <v>1</v>
-      </c>
-      <c r="E37" s="23"/>
+      <c r="D37" s="25">
+        <v>1</v>
+      </c>
+      <c r="E37" s="28"/>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="20"/>
+      <c r="A38" s="24"/>
       <c r="B38" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="20"/>
-      <c r="D38" s="32"/>
-      <c r="E38" s="32"/>
+      <c r="C38" s="24"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="26"/>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="20"/>
+      <c r="A39" s="24"/>
       <c r="B39" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C39" s="20"/>
-      <c r="D39" s="32"/>
-      <c r="E39" s="32"/>
+      <c r="C39" s="24"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="26"/>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="20"/>
+      <c r="A40" s="24"/>
       <c r="B40" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
+      <c r="C40" s="24"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="6">
@@ -1293,20 +1291,20 @@
       <c r="E41" s="6"/>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="31" t="s">
+      <c r="A42" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="B42" s="31"/>
-      <c r="C42" s="31"/>
-      <c r="D42" s="31"/>
-      <c r="E42" s="31"/>
+      <c r="B42" s="23"/>
+      <c r="C42" s="23"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="23"/>
       <c r="F42">
         <f>SUM(C43:C45)</f>
         <v>1.5</v>
       </c>
       <c r="G42">
         <f>C43*D43+C44*D44+C45*D45</f>
-        <v>0</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -1320,7 +1318,7 @@
         <v>0.5</v>
       </c>
       <c r="D43" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E43" s="6"/>
     </row>
@@ -1335,7 +1333,7 @@
         <v>0.5</v>
       </c>
       <c r="D44" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E44" s="6"/>
     </row>
@@ -1350,143 +1348,170 @@
         <v>0.5</v>
       </c>
       <c r="D45" s="8">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E45" s="6"/>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="31" t="s">
+      <c r="A46" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="B46" s="31"/>
-      <c r="C46" s="31"/>
-      <c r="D46" s="31"/>
-      <c r="E46" s="31"/>
+      <c r="B46" s="23"/>
+      <c r="C46" s="23"/>
+      <c r="D46" s="23"/>
+      <c r="E46" s="23"/>
       <c r="F46">
         <f>SUM(C47:C55)</f>
         <v>2.75</v>
       </c>
       <c r="G46">
         <f>C47*D47+C50*D50+C52*D52+C54*D54</f>
-        <v>1.375</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="20">
+      <c r="A47" s="24">
         <v>4.0999999999999996</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C47" s="20">
+      <c r="C47" s="24">
         <v>0.5</v>
       </c>
-      <c r="D47" s="21">
-        <v>0.25</v>
-      </c>
-      <c r="E47" s="23"/>
+      <c r="D47" s="25">
+        <v>1</v>
+      </c>
+      <c r="E47" s="28"/>
     </row>
     <row r="48" spans="1:7">
-      <c r="A48" s="20"/>
+      <c r="A48" s="24"/>
       <c r="B48" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C48" s="20"/>
-      <c r="D48" s="32"/>
-      <c r="E48" s="32"/>
+      <c r="C48" s="24"/>
+      <c r="D48" s="26"/>
+      <c r="E48" s="26"/>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" s="20"/>
+      <c r="A49" s="24"/>
       <c r="B49" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C49" s="20"/>
-      <c r="D49" s="22"/>
-      <c r="E49" s="22"/>
+      <c r="C49" s="24"/>
+      <c r="D49" s="27"/>
+      <c r="E49" s="27"/>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="20">
+      <c r="A50" s="24">
         <v>4.2</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C50" s="20">
-        <v>1</v>
-      </c>
-      <c r="D50" s="29">
+      <c r="C50" s="24">
+        <v>1</v>
+      </c>
+      <c r="D50" s="32">
         <v>0</v>
       </c>
-      <c r="E50" s="23"/>
+      <c r="E50" s="28"/>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="20"/>
+      <c r="A51" s="24"/>
       <c r="B51" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C51" s="20"/>
-      <c r="D51" s="30"/>
-      <c r="E51" s="22"/>
+      <c r="C51" s="24"/>
+      <c r="D51" s="33"/>
+      <c r="E51" s="27"/>
     </row>
     <row r="52" spans="1:6">
-      <c r="A52" s="20">
+      <c r="A52" s="24">
         <v>4.3</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C52" s="20">
+      <c r="C52" s="24">
         <v>0.5</v>
       </c>
-      <c r="D52" s="29">
-        <v>1</v>
-      </c>
-      <c r="E52" s="23"/>
+      <c r="D52" s="32">
+        <v>1</v>
+      </c>
+      <c r="E52" s="28"/>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="20"/>
+      <c r="A53" s="24"/>
       <c r="B53" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C53" s="20"/>
-      <c r="D53" s="30"/>
-      <c r="E53" s="22"/>
+      <c r="C53" s="24"/>
+      <c r="D53" s="33"/>
+      <c r="E53" s="27"/>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="20">
+      <c r="A54" s="24">
         <v>4.4000000000000004</v>
       </c>
       <c r="B54" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C54" s="20">
+      <c r="C54" s="24">
         <v>0.75</v>
       </c>
-      <c r="D54" s="21">
-        <v>1</v>
-      </c>
-      <c r="E54" s="23"/>
+      <c r="D54" s="25">
+        <v>1</v>
+      </c>
+      <c r="E54" s="28"/>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="20"/>
+      <c r="A55" s="24"/>
       <c r="B55" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C55" s="20"/>
-      <c r="D55" s="22"/>
-      <c r="E55" s="22"/>
+      <c r="C55" s="24"/>
+      <c r="D55" s="27"/>
+      <c r="E55" s="27"/>
     </row>
     <row r="57" spans="1:6">
       <c r="F57" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="C13:C16"/>
-    <mergeCell ref="D13:D16"/>
-    <mergeCell ref="E13:E16"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="E50:E51"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="A42:E42"/>
+    <mergeCell ref="A46:E46"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="E28:E31"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="D47:D49"/>
+    <mergeCell ref="E47:E49"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="E34:E36"/>
+    <mergeCell ref="A37:A40"/>
+    <mergeCell ref="C37:C40"/>
+    <mergeCell ref="D37:D40"/>
+    <mergeCell ref="E37:E40"/>
     <mergeCell ref="A32:A33"/>
     <mergeCell ref="C32:C33"/>
     <mergeCell ref="D32:D33"/>
@@ -1503,39 +1528,12 @@
     <mergeCell ref="A28:A31"/>
     <mergeCell ref="C28:C31"/>
     <mergeCell ref="D28:D31"/>
-    <mergeCell ref="E28:E31"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="D47:D49"/>
-    <mergeCell ref="E47:E49"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="C34:C36"/>
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="E34:E36"/>
-    <mergeCell ref="A37:A40"/>
-    <mergeCell ref="C37:C40"/>
-    <mergeCell ref="D37:D40"/>
-    <mergeCell ref="E37:E40"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="E50:E51"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="A42:E42"/>
-    <mergeCell ref="A46:E46"/>
-    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="D13:D16"/>
+    <mergeCell ref="E13:E16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Cập nhật lại Phieu van dap.xlsx
</commit_message>
<xml_diff>
--- a/+ Ban nop/Phieu van dap.xlsx
+++ b/+ Ban nop/Phieu van dap.xlsx
@@ -459,18 +459,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -481,21 +496,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -796,7 +796,7 @@
   <dimension ref="A1:H57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17:D22"/>
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -814,12 +814,12 @@
       <c r="A1" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="19" t="s">
@@ -831,10 +831,10 @@
       <c r="C2" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="E2" s="26"/>
+      <c r="E2" s="31"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="18" t="s">
@@ -846,8 +846,8 @@
       <c r="C3" s="20">
         <v>0.9</v>
       </c>
-      <c r="D3" s="31"/>
-      <c r="E3" s="32"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="27"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="18" t="s">
@@ -859,8 +859,8 @@
       <c r="C4" s="20">
         <v>0.89</v>
       </c>
-      <c r="D4" s="31"/>
-      <c r="E4" s="32"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="27"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="18" t="s">
@@ -872,8 +872,8 @@
       <c r="C5" s="20">
         <v>0.97</v>
       </c>
-      <c r="D5" s="31"/>
-      <c r="E5" s="32"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="27"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="18" t="s">
@@ -885,8 +885,8 @@
       <c r="C6" s="20">
         <v>0.97</v>
       </c>
-      <c r="D6" s="31"/>
-      <c r="E6" s="32"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="27"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="18" t="s">
@@ -898,8 +898,8 @@
       <c r="C7" s="20">
         <v>0.99</v>
       </c>
-      <c r="D7" s="31"/>
-      <c r="E7" s="32"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="27"/>
     </row>
     <row r="9" spans="1:8" ht="31.5">
       <c r="A9" s="11" t="s">
@@ -945,21 +945,21 @@
       </c>
       <c r="G11">
         <f>SUM(G12,G27,G42,G46)</f>
-        <v>11</v>
+        <v>10.5</v>
       </c>
       <c r="H11">
         <f>G11*3.75/10</f>
-        <v>4.125</v>
+        <v>3.9375</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="29"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
       <c r="F12">
         <f>SUM(C13:C26)</f>
         <v>3.25</v>
@@ -970,139 +970,139 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="21">
+      <c r="A13" s="22">
         <v>1.1000000000000001</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="21">
+      <c r="C13" s="22">
         <v>0.75</v>
       </c>
-      <c r="D13" s="22">
-        <v>1</v>
-      </c>
-      <c r="E13" s="24"/>
+      <c r="D13" s="23">
+        <v>1</v>
+      </c>
+      <c r="E13" s="28"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="21"/>
+      <c r="A14" s="22"/>
       <c r="B14" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="21"/>
+      <c r="A15" s="22"/>
       <c r="B15" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="21"/>
+      <c r="A16" s="22"/>
       <c r="B16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="21">
+      <c r="A17" s="22">
         <v>1.2</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="21">
-        <v>1</v>
-      </c>
-      <c r="D17" s="22">
-        <v>1</v>
-      </c>
-      <c r="E17" s="24"/>
+      <c r="C17" s="22">
+        <v>1</v>
+      </c>
+      <c r="D17" s="23">
+        <v>1</v>
+      </c>
+      <c r="E17" s="28"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="21"/>
+      <c r="A18" s="22"/>
       <c r="B18" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="21"/>
+      <c r="A19" s="22"/>
       <c r="B19" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="21"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="21"/>
+      <c r="A20" s="22"/>
       <c r="B20" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="21"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="21"/>
+      <c r="A21" s="22"/>
       <c r="B21" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="21"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="21"/>
+      <c r="A22" s="22"/>
       <c r="B22" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="21"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="21">
+      <c r="A23" s="22">
         <v>1.3</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="21">
-        <v>1</v>
-      </c>
-      <c r="D23" s="22">
+      <c r="C23" s="22">
+        <v>1</v>
+      </c>
+      <c r="D23" s="23">
         <v>0.75</v>
       </c>
-      <c r="E23" s="24"/>
+      <c r="E23" s="28"/>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="21"/>
+      <c r="A24" s="22"/>
       <c r="B24" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="21"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="21"/>
+      <c r="A25" s="22"/>
       <c r="B25" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="21"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="6">
@@ -1120,13 +1120,13 @@
       <c r="E26" s="6"/>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="29" t="s">
+      <c r="A27" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
       <c r="F27">
         <f>SUM(C28:C41)</f>
         <v>4</v>
@@ -1137,145 +1137,145 @@
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="21">
+      <c r="A28" s="22">
         <v>2.1</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="21">
+      <c r="C28" s="22">
         <v>0.75</v>
       </c>
-      <c r="D28" s="22">
-        <v>1</v>
-      </c>
-      <c r="E28" s="24"/>
+      <c r="D28" s="23">
+        <v>1</v>
+      </c>
+      <c r="E28" s="28"/>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="21"/>
+      <c r="A29" s="22"/>
       <c r="B29" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="21"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="33"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="24"/>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="21"/>
+      <c r="A30" s="22"/>
       <c r="B30" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="21"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="21"/>
+      <c r="A31" s="22"/>
       <c r="B31" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="21"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="25"/>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="21">
+      <c r="A32" s="22">
         <v>2.2000000000000002</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="21">
+      <c r="C32" s="22">
         <v>0.5</v>
       </c>
-      <c r="D32" s="22">
-        <v>1</v>
-      </c>
-      <c r="E32" s="24"/>
+      <c r="D32" s="23">
+        <v>1</v>
+      </c>
+      <c r="E32" s="28"/>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="21"/>
+      <c r="A33" s="22"/>
       <c r="B33" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="21"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="25"/>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="21">
+      <c r="A34" s="22">
         <v>2.2999999999999998</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="21">
+      <c r="C34" s="22">
         <v>0.75</v>
       </c>
-      <c r="D34" s="22">
-        <v>1</v>
-      </c>
-      <c r="E34" s="24"/>
+      <c r="D34" s="23">
+        <v>1</v>
+      </c>
+      <c r="E34" s="28"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="21"/>
+      <c r="A35" s="22"/>
       <c r="B35" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="21"/>
-      <c r="D35" s="33"/>
-      <c r="E35" s="33"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="21"/>
+      <c r="A36" s="22"/>
       <c r="B36" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="21"/>
-      <c r="D36" s="23"/>
-      <c r="E36" s="23"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="25"/>
+      <c r="E36" s="25"/>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="21">
+      <c r="A37" s="22">
         <v>2.4</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C37" s="21">
+      <c r="C37" s="22">
         <v>1.5</v>
       </c>
-      <c r="D37" s="22">
-        <v>1</v>
-      </c>
-      <c r="E37" s="24"/>
+      <c r="D37" s="23">
+        <v>1</v>
+      </c>
+      <c r="E37" s="28"/>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="21"/>
+      <c r="A38" s="22"/>
       <c r="B38" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="21"/>
-      <c r="D38" s="33"/>
-      <c r="E38" s="33"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="24"/>
+      <c r="E38" s="24"/>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="21"/>
+      <c r="A39" s="22"/>
       <c r="B39" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C39" s="21"/>
-      <c r="D39" s="33"/>
-      <c r="E39" s="33"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="24"/>
+      <c r="E39" s="24"/>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="21"/>
+      <c r="A40" s="22"/>
       <c r="B40" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C40" s="21"/>
-      <c r="D40" s="23"/>
-      <c r="E40" s="23"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="25"/>
+      <c r="E40" s="25"/>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="6">
@@ -1293,13 +1293,13 @@
       <c r="E41" s="6"/>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="29" t="s">
+      <c r="A42" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="B42" s="29"/>
-      <c r="C42" s="29"/>
-      <c r="D42" s="29"/>
-      <c r="E42" s="29"/>
+      <c r="B42" s="21"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
       <c r="F42">
         <f>SUM(C43:C45)</f>
         <v>1.5</v>
@@ -1355,132 +1355,171 @@
       <c r="E45" s="6"/>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="29" t="s">
+      <c r="A46" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="B46" s="29"/>
-      <c r="C46" s="29"/>
-      <c r="D46" s="29"/>
-      <c r="E46" s="29"/>
+      <c r="B46" s="21"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="21"/>
+      <c r="E46" s="21"/>
       <c r="F46">
         <f>SUM(C47:C55)</f>
         <v>2.75</v>
       </c>
       <c r="G46">
         <f>C47*D47+C50*D50+C52*D52+C54*D54</f>
-        <v>2.75</v>
+        <v>2.25</v>
       </c>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="21">
+      <c r="A47" s="22">
         <v>4.0999999999999996</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C47" s="21">
+      <c r="C47" s="22">
         <v>0.5</v>
       </c>
-      <c r="D47" s="22">
-        <v>1</v>
-      </c>
-      <c r="E47" s="24"/>
+      <c r="D47" s="23">
+        <v>1</v>
+      </c>
+      <c r="E47" s="28"/>
     </row>
     <row r="48" spans="1:7">
-      <c r="A48" s="21"/>
+      <c r="A48" s="22"/>
       <c r="B48" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C48" s="21"/>
-      <c r="D48" s="33"/>
-      <c r="E48" s="33"/>
+      <c r="C48" s="22"/>
+      <c r="D48" s="24"/>
+      <c r="E48" s="24"/>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" s="21"/>
+      <c r="A49" s="22"/>
       <c r="B49" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C49" s="21"/>
-      <c r="D49" s="23"/>
-      <c r="E49" s="23"/>
+      <c r="C49" s="22"/>
+      <c r="D49" s="25"/>
+      <c r="E49" s="25"/>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="21">
+      <c r="A50" s="22">
         <v>4.2</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C50" s="21">
-        <v>1</v>
-      </c>
-      <c r="D50" s="27">
-        <v>1</v>
-      </c>
-      <c r="E50" s="24"/>
+      <c r="C50" s="22">
+        <v>1</v>
+      </c>
+      <c r="D50" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="E50" s="28"/>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="21"/>
+      <c r="A51" s="22"/>
       <c r="B51" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C51" s="21"/>
-      <c r="D51" s="28"/>
-      <c r="E51" s="23"/>
+      <c r="C51" s="22"/>
+      <c r="D51" s="33"/>
+      <c r="E51" s="25"/>
     </row>
     <row r="52" spans="1:6">
-      <c r="A52" s="21">
+      <c r="A52" s="22">
         <v>4.3</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C52" s="21">
+      <c r="C52" s="22">
         <v>0.5</v>
       </c>
-      <c r="D52" s="27">
-        <v>1</v>
-      </c>
-      <c r="E52" s="24"/>
+      <c r="D52" s="32">
+        <v>1</v>
+      </c>
+      <c r="E52" s="28"/>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="21"/>
+      <c r="A53" s="22"/>
       <c r="B53" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C53" s="21"/>
-      <c r="D53" s="28"/>
-      <c r="E53" s="23"/>
+      <c r="C53" s="22"/>
+      <c r="D53" s="33"/>
+      <c r="E53" s="25"/>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="21">
+      <c r="A54" s="22">
         <v>4.4000000000000004</v>
       </c>
       <c r="B54" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C54" s="21">
+      <c r="C54" s="22">
         <v>0.75</v>
       </c>
-      <c r="D54" s="22">
-        <v>1</v>
-      </c>
-      <c r="E54" s="24"/>
+      <c r="D54" s="23">
+        <v>1</v>
+      </c>
+      <c r="E54" s="28"/>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="21"/>
+      <c r="A55" s="22"/>
       <c r="B55" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C55" s="21"/>
-      <c r="D55" s="23"/>
-      <c r="E55" s="23"/>
+      <c r="C55" s="22"/>
+      <c r="D55" s="25"/>
+      <c r="E55" s="25"/>
     </row>
     <row r="57" spans="1:6">
       <c r="F57" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="E50:E51"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="A42:E42"/>
+    <mergeCell ref="A46:E46"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="E34:E36"/>
+    <mergeCell ref="A37:A40"/>
+    <mergeCell ref="C37:C40"/>
+    <mergeCell ref="D37:D40"/>
+    <mergeCell ref="E37:E40"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="E23:E25"/>
+    <mergeCell ref="E28:E31"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="D47:D49"/>
+    <mergeCell ref="E47:E49"/>
     <mergeCell ref="A27:E27"/>
     <mergeCell ref="A28:A31"/>
     <mergeCell ref="C28:C31"/>
@@ -1497,45 +1536,6 @@
     <mergeCell ref="E17:E22"/>
     <mergeCell ref="A23:A25"/>
     <mergeCell ref="C23:C25"/>
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="E23:E25"/>
-    <mergeCell ref="E28:E31"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="D47:D49"/>
-    <mergeCell ref="E47:E49"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="C34:C36"/>
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="E34:E36"/>
-    <mergeCell ref="A37:A40"/>
-    <mergeCell ref="C37:C40"/>
-    <mergeCell ref="D37:D40"/>
-    <mergeCell ref="E37:E40"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="E50:E51"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="A42:E42"/>
-    <mergeCell ref="A46:E46"/>
-    <mergeCell ref="A47:A49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
update lại phát tán tin rao vặt. ông Thuận nõi là làm được 100%
</commit_message>
<xml_diff>
--- a/+ Ban nop/Phieu van dap.xlsx
+++ b/+ Ban nop/Phieu van dap.xlsx
@@ -459,20 +459,35 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -480,22 +495,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -795,8 +795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -814,12 +814,12 @@
       <c r="A1" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="19" t="s">
@@ -831,10 +831,10 @@
       <c r="C2" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="E2" s="31"/>
+      <c r="E2" s="26"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="18" t="s">
@@ -846,8 +846,8 @@
       <c r="C3" s="20">
         <v>0.9</v>
       </c>
-      <c r="D3" s="26"/>
-      <c r="E3" s="27"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="32"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="18" t="s">
@@ -859,8 +859,8 @@
       <c r="C4" s="20">
         <v>0.89</v>
       </c>
-      <c r="D4" s="26"/>
-      <c r="E4" s="27"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="32"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="18" t="s">
@@ -872,8 +872,8 @@
       <c r="C5" s="20">
         <v>0.97</v>
       </c>
-      <c r="D5" s="26"/>
-      <c r="E5" s="27"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="32"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="18" t="s">
@@ -885,8 +885,8 @@
       <c r="C6" s="20">
         <v>0.97</v>
       </c>
-      <c r="D6" s="26"/>
-      <c r="E6" s="27"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="32"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="18" t="s">
@@ -898,8 +898,8 @@
       <c r="C7" s="20">
         <v>0.99</v>
       </c>
-      <c r="D7" s="26"/>
-      <c r="E7" s="27"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="32"/>
     </row>
     <row r="9" spans="1:8" ht="31.5">
       <c r="A9" s="11" t="s">
@@ -945,21 +945,21 @@
       </c>
       <c r="G11">
         <f>SUM(G12,G27,G42,G46)</f>
-        <v>10.5</v>
+        <v>10.75</v>
       </c>
       <c r="H11">
         <f>G11*3.75/10</f>
-        <v>3.9375</v>
+        <v>4.03125</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
       <c r="F12">
         <f>SUM(C13:C26)</f>
         <v>3.25</v>
@@ -970,139 +970,139 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="22">
+      <c r="A13" s="21">
         <v>1.1000000000000001</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="22">
+      <c r="C13" s="21">
         <v>0.75</v>
       </c>
-      <c r="D13" s="23">
-        <v>1</v>
-      </c>
-      <c r="E13" s="28"/>
+      <c r="D13" s="22">
+        <v>1</v>
+      </c>
+      <c r="E13" s="24"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="22"/>
+      <c r="A14" s="21"/>
       <c r="B14" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="22"/>
+      <c r="A15" s="21"/>
       <c r="B15" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="22"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="22"/>
+      <c r="A16" s="21"/>
       <c r="B16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="22">
+      <c r="A17" s="21">
         <v>1.2</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="22">
-        <v>1</v>
-      </c>
-      <c r="D17" s="23">
-        <v>1</v>
-      </c>
-      <c r="E17" s="28"/>
+      <c r="C17" s="21">
+        <v>1</v>
+      </c>
+      <c r="D17" s="22">
+        <v>1</v>
+      </c>
+      <c r="E17" s="24"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="22"/>
+      <c r="A18" s="21"/>
       <c r="B18" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="22"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="22"/>
+      <c r="A19" s="21"/>
       <c r="B19" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="22"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="22"/>
+      <c r="A20" s="21"/>
       <c r="B20" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="22"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="22"/>
+      <c r="A21" s="21"/>
       <c r="B21" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="22"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="22"/>
+      <c r="A22" s="21"/>
       <c r="B22" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="22"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="22">
+      <c r="A23" s="21">
         <v>1.3</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="22">
-        <v>1</v>
-      </c>
-      <c r="D23" s="23">
+      <c r="C23" s="21">
+        <v>1</v>
+      </c>
+      <c r="D23" s="22">
         <v>0.75</v>
       </c>
-      <c r="E23" s="28"/>
+      <c r="E23" s="24"/>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="22"/>
+      <c r="A24" s="21"/>
       <c r="B24" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="22"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="22"/>
+      <c r="A25" s="21"/>
       <c r="B25" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="22"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="6">
@@ -1120,13 +1120,13 @@
       <c r="E26" s="6"/>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="21" t="s">
+      <c r="A27" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
       <c r="F27">
         <f>SUM(C28:C41)</f>
         <v>4</v>
@@ -1137,145 +1137,145 @@
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="22">
+      <c r="A28" s="21">
         <v>2.1</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="22">
+      <c r="C28" s="21">
         <v>0.75</v>
       </c>
-      <c r="D28" s="23">
-        <v>1</v>
-      </c>
-      <c r="E28" s="28"/>
+      <c r="D28" s="22">
+        <v>1</v>
+      </c>
+      <c r="E28" s="24"/>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="22"/>
+      <c r="A29" s="21"/>
       <c r="B29" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="22"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="24"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="33"/>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="22"/>
+      <c r="A30" s="21"/>
       <c r="B30" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="22"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="22"/>
+      <c r="A31" s="21"/>
       <c r="B31" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="22"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="22">
+      <c r="A32" s="21">
         <v>2.2000000000000002</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="22">
+      <c r="C32" s="21">
         <v>0.5</v>
       </c>
-      <c r="D32" s="23">
-        <v>1</v>
-      </c>
-      <c r="E32" s="28"/>
+      <c r="D32" s="22">
+        <v>1</v>
+      </c>
+      <c r="E32" s="24"/>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="22"/>
+      <c r="A33" s="21"/>
       <c r="B33" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="22"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23"/>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="22">
+      <c r="A34" s="21">
         <v>2.2999999999999998</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="22">
+      <c r="C34" s="21">
         <v>0.75</v>
       </c>
-      <c r="D34" s="23">
-        <v>1</v>
-      </c>
-      <c r="E34" s="28"/>
+      <c r="D34" s="22">
+        <v>1</v>
+      </c>
+      <c r="E34" s="24"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="22"/>
+      <c r="A35" s="21"/>
       <c r="B35" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="22"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="24"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="33"/>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="22"/>
+      <c r="A36" s="21"/>
       <c r="B36" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="22"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="25"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="23"/>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="22">
+      <c r="A37" s="21">
         <v>2.4</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C37" s="22">
+      <c r="C37" s="21">
         <v>1.5</v>
       </c>
-      <c r="D37" s="23">
-        <v>1</v>
-      </c>
-      <c r="E37" s="28"/>
+      <c r="D37" s="22">
+        <v>1</v>
+      </c>
+      <c r="E37" s="24"/>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="22"/>
+      <c r="A38" s="21"/>
       <c r="B38" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="22"/>
-      <c r="D38" s="24"/>
-      <c r="E38" s="24"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="33"/>
+      <c r="E38" s="33"/>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="22"/>
+      <c r="A39" s="21"/>
       <c r="B39" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C39" s="22"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="24"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="33"/>
+      <c r="E39" s="33"/>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="22"/>
+      <c r="A40" s="21"/>
       <c r="B40" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C40" s="22"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="25"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="23"/>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="6">
@@ -1293,20 +1293,20 @@
       <c r="E41" s="6"/>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="B42" s="21"/>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
+      <c r="B42" s="29"/>
+      <c r="C42" s="29"/>
+      <c r="D42" s="29"/>
+      <c r="E42" s="29"/>
       <c r="F42">
         <f>SUM(C43:C45)</f>
         <v>1.5</v>
       </c>
       <c r="G42">
         <f>C43*D43+C44*D44+C45*D45</f>
-        <v>1.25</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -1350,18 +1350,18 @@
         <v>0.5</v>
       </c>
       <c r="D45" s="8">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E45" s="6"/>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="21" t="s">
+      <c r="A46" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="B46" s="21"/>
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
-      <c r="E46" s="21"/>
+      <c r="B46" s="29"/>
+      <c r="C46" s="29"/>
+      <c r="D46" s="29"/>
+      <c r="E46" s="29"/>
       <c r="F46">
         <f>SUM(C47:C55)</f>
         <v>2.75</v>
@@ -1372,115 +1372,154 @@
       </c>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="22">
+      <c r="A47" s="21">
         <v>4.0999999999999996</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C47" s="22">
+      <c r="C47" s="21">
         <v>0.5</v>
       </c>
-      <c r="D47" s="23">
-        <v>1</v>
-      </c>
-      <c r="E47" s="28"/>
+      <c r="D47" s="22">
+        <v>1</v>
+      </c>
+      <c r="E47" s="24"/>
     </row>
     <row r="48" spans="1:7">
-      <c r="A48" s="22"/>
+      <c r="A48" s="21"/>
       <c r="B48" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C48" s="22"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="24"/>
+      <c r="C48" s="21"/>
+      <c r="D48" s="33"/>
+      <c r="E48" s="33"/>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" s="22"/>
+      <c r="A49" s="21"/>
       <c r="B49" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C49" s="22"/>
-      <c r="D49" s="25"/>
-      <c r="E49" s="25"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="23"/>
+      <c r="E49" s="23"/>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="22">
+      <c r="A50" s="21">
         <v>4.2</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C50" s="22">
-        <v>1</v>
-      </c>
-      <c r="D50" s="32">
+      <c r="C50" s="21">
+        <v>1</v>
+      </c>
+      <c r="D50" s="27">
         <v>0.5</v>
       </c>
-      <c r="E50" s="28"/>
+      <c r="E50" s="24"/>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="22"/>
+      <c r="A51" s="21"/>
       <c r="B51" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C51" s="22"/>
-      <c r="D51" s="33"/>
-      <c r="E51" s="25"/>
+      <c r="C51" s="21"/>
+      <c r="D51" s="28"/>
+      <c r="E51" s="23"/>
     </row>
     <row r="52" spans="1:6">
-      <c r="A52" s="22">
+      <c r="A52" s="21">
         <v>4.3</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C52" s="22">
+      <c r="C52" s="21">
         <v>0.5</v>
       </c>
-      <c r="D52" s="32">
-        <v>1</v>
-      </c>
-      <c r="E52" s="28"/>
+      <c r="D52" s="27">
+        <v>1</v>
+      </c>
+      <c r="E52" s="24"/>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="22"/>
+      <c r="A53" s="21"/>
       <c r="B53" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C53" s="22"/>
-      <c r="D53" s="33"/>
-      <c r="E53" s="25"/>
+      <c r="C53" s="21"/>
+      <c r="D53" s="28"/>
+      <c r="E53" s="23"/>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="22">
+      <c r="A54" s="21">
         <v>4.4000000000000004</v>
       </c>
       <c r="B54" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C54" s="22">
+      <c r="C54" s="21">
         <v>0.75</v>
       </c>
-      <c r="D54" s="23">
-        <v>1</v>
-      </c>
-      <c r="E54" s="28"/>
+      <c r="D54" s="22">
+        <v>1</v>
+      </c>
+      <c r="E54" s="24"/>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="22"/>
+      <c r="A55" s="21"/>
       <c r="B55" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C55" s="22"/>
-      <c r="D55" s="25"/>
-      <c r="E55" s="25"/>
+      <c r="C55" s="21"/>
+      <c r="D55" s="23"/>
+      <c r="E55" s="23"/>
     </row>
     <row r="57" spans="1:6">
       <c r="F57" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="D13:D16"/>
+    <mergeCell ref="E13:E16"/>
+    <mergeCell ref="A17:A22"/>
+    <mergeCell ref="C17:C22"/>
+    <mergeCell ref="D17:D22"/>
+    <mergeCell ref="E17:E22"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="D47:D49"/>
+    <mergeCell ref="E47:E49"/>
+    <mergeCell ref="A27:E27"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="E34:E36"/>
+    <mergeCell ref="A37:A40"/>
+    <mergeCell ref="C37:C40"/>
+    <mergeCell ref="D37:D40"/>
+    <mergeCell ref="E37:E40"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="E23:E25"/>
+    <mergeCell ref="E28:E31"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="C13:C16"/>
     <mergeCell ref="A54:A55"/>
     <mergeCell ref="C54:C55"/>
     <mergeCell ref="D54:D55"/>
@@ -1497,45 +1536,6 @@
     <mergeCell ref="A42:E42"/>
     <mergeCell ref="A46:E46"/>
     <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="C34:C36"/>
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="E34:E36"/>
-    <mergeCell ref="A37:A40"/>
-    <mergeCell ref="C37:C40"/>
-    <mergeCell ref="D37:D40"/>
-    <mergeCell ref="E37:E40"/>
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="E23:E25"/>
-    <mergeCell ref="E28:E31"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="D47:D49"/>
-    <mergeCell ref="E47:E49"/>
-    <mergeCell ref="A27:E27"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="C28:C31"/>
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="C13:C16"/>
-    <mergeCell ref="D13:D16"/>
-    <mergeCell ref="E13:E16"/>
-    <mergeCell ref="A17:A22"/>
-    <mergeCell ref="C17:C22"/>
-    <mergeCell ref="D17:D22"/>
-    <mergeCell ref="E17:E22"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="C23:C25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Cập nhật bản nộp. Bản chính thức, build không bị lỗi.
</commit_message>
<xml_diff>
--- a/+ Ban nop/Phieu van dap.xlsx
+++ b/+ Ban nop/Phieu van dap.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="PhieuVanDap" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -465,12 +465,27 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -481,21 +496,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -795,9 +795,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -814,12 +812,12 @@
       <c r="A1" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="19" t="s">
@@ -831,10 +829,10 @@
       <c r="C2" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="E2" s="26"/>
+      <c r="E2" s="31"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="18" t="s">
@@ -846,8 +844,8 @@
       <c r="C3" s="20">
         <v>0.9</v>
       </c>
-      <c r="D3" s="31"/>
-      <c r="E3" s="32"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="29"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="18" t="s">
@@ -859,8 +857,8 @@
       <c r="C4" s="20">
         <v>0.89</v>
       </c>
-      <c r="D4" s="31"/>
-      <c r="E4" s="32"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="29"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="18" t="s">
@@ -872,8 +870,8 @@
       <c r="C5" s="20">
         <v>0.97</v>
       </c>
-      <c r="D5" s="31"/>
-      <c r="E5" s="32"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="29"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="18" t="s">
@@ -885,8 +883,8 @@
       <c r="C6" s="20">
         <v>0.97</v>
       </c>
-      <c r="D6" s="31"/>
-      <c r="E6" s="32"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="29"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="18" t="s">
@@ -898,8 +896,8 @@
       <c r="C7" s="20">
         <v>0.99</v>
       </c>
-      <c r="D7" s="31"/>
-      <c r="E7" s="32"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="29"/>
     </row>
     <row r="9" spans="1:8" ht="31.5">
       <c r="A9" s="11" t="s">
@@ -945,21 +943,21 @@
       </c>
       <c r="G11">
         <f>SUM(G12,G27,G42,G46)</f>
-        <v>10.75</v>
+        <v>10.225</v>
       </c>
       <c r="H11">
         <f>G11*3.75/10</f>
-        <v>4.03125</v>
+        <v>3.8343750000000001</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="29"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
       <c r="F12">
         <f>SUM(C13:C26)</f>
         <v>3.25</v>
@@ -982,7 +980,7 @@
       <c r="D13" s="22">
         <v>1</v>
       </c>
-      <c r="E13" s="24"/>
+      <c r="E13" s="25"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="21"/>
@@ -990,8 +988,8 @@
         <v>10</v>
       </c>
       <c r="C14" s="21"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="21"/>
@@ -999,8 +997,8 @@
         <v>11</v>
       </c>
       <c r="C15" s="21"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="21"/>
@@ -1008,8 +1006,8 @@
         <v>12</v>
       </c>
       <c r="C16" s="21"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="21">
@@ -1024,7 +1022,7 @@
       <c r="D17" s="22">
         <v>1</v>
       </c>
-      <c r="E17" s="24"/>
+      <c r="E17" s="25"/>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="21"/>
@@ -1032,8 +1030,8 @@
         <v>14</v>
       </c>
       <c r="C18" s="21"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="21"/>
@@ -1041,8 +1039,8 @@
         <v>15</v>
       </c>
       <c r="C19" s="21"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="21"/>
@@ -1050,8 +1048,8 @@
         <v>16</v>
       </c>
       <c r="C20" s="21"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="21"/>
@@ -1059,8 +1057,8 @@
         <v>17</v>
       </c>
       <c r="C21" s="21"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="21"/>
@@ -1068,8 +1066,8 @@
         <v>18</v>
       </c>
       <c r="C22" s="21"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="21">
@@ -1084,7 +1082,7 @@
       <c r="D23" s="22">
         <v>0.75</v>
       </c>
-      <c r="E23" s="24"/>
+      <c r="E23" s="25"/>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="21"/>
@@ -1092,8 +1090,8 @@
         <v>20</v>
       </c>
       <c r="C24" s="21"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="21"/>
@@ -1101,8 +1099,8 @@
         <v>21</v>
       </c>
       <c r="C25" s="21"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="6">
@@ -1120,13 +1118,13 @@
       <c r="E26" s="6"/>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="29" t="s">
+      <c r="A27" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
       <c r="F27">
         <f>SUM(C28:C41)</f>
         <v>4</v>
@@ -1149,7 +1147,7 @@
       <c r="D28" s="22">
         <v>1</v>
       </c>
-      <c r="E28" s="24"/>
+      <c r="E28" s="25"/>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="21"/>
@@ -1157,8 +1155,8 @@
         <v>25</v>
       </c>
       <c r="C29" s="21"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="33"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="21"/>
@@ -1166,8 +1164,8 @@
         <v>26</v>
       </c>
       <c r="C30" s="21"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="21"/>
@@ -1175,8 +1173,8 @@
         <v>27</v>
       </c>
       <c r="C31" s="21"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="21">
@@ -1191,7 +1189,7 @@
       <c r="D32" s="22">
         <v>1</v>
       </c>
-      <c r="E32" s="24"/>
+      <c r="E32" s="25"/>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="21"/>
@@ -1199,8 +1197,8 @@
         <v>29</v>
       </c>
       <c r="C33" s="21"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="21">
@@ -1215,7 +1213,7 @@
       <c r="D34" s="22">
         <v>1</v>
       </c>
-      <c r="E34" s="24"/>
+      <c r="E34" s="25"/>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="21"/>
@@ -1223,8 +1221,8 @@
         <v>31</v>
       </c>
       <c r="C35" s="21"/>
-      <c r="D35" s="33"/>
-      <c r="E35" s="33"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="23"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="21"/>
@@ -1232,8 +1230,8 @@
         <v>32</v>
       </c>
       <c r="C36" s="21"/>
-      <c r="D36" s="23"/>
-      <c r="E36" s="23"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="21">
@@ -1248,7 +1246,7 @@
       <c r="D37" s="22">
         <v>1</v>
       </c>
-      <c r="E37" s="24"/>
+      <c r="E37" s="25"/>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="21"/>
@@ -1256,8 +1254,8 @@
         <v>34</v>
       </c>
       <c r="C38" s="21"/>
-      <c r="D38" s="33"/>
-      <c r="E38" s="33"/>
+      <c r="D38" s="23"/>
+      <c r="E38" s="23"/>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="21"/>
@@ -1265,8 +1263,8 @@
         <v>35</v>
       </c>
       <c r="C39" s="21"/>
-      <c r="D39" s="33"/>
-      <c r="E39" s="33"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="23"/>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="21"/>
@@ -1274,8 +1272,8 @@
         <v>36</v>
       </c>
       <c r="C40" s="21"/>
-      <c r="D40" s="23"/>
-      <c r="E40" s="23"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="24"/>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="6">
@@ -1293,20 +1291,20 @@
       <c r="E41" s="6"/>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="29" t="s">
+      <c r="A42" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="B42" s="29"/>
-      <c r="C42" s="29"/>
-      <c r="D42" s="29"/>
-      <c r="E42" s="29"/>
+      <c r="B42" s="26"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="26"/>
       <c r="F42">
         <f>SUM(C43:C45)</f>
         <v>1.5</v>
       </c>
       <c r="G42">
         <f>C43*D43+C44*D44+C45*D45</f>
-        <v>1.5</v>
+        <v>1.375</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -1350,25 +1348,25 @@
         <v>0.5</v>
       </c>
       <c r="D45" s="8">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="E45" s="6"/>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="29" t="s">
+      <c r="A46" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="B46" s="29"/>
-      <c r="C46" s="29"/>
-      <c r="D46" s="29"/>
-      <c r="E46" s="29"/>
+      <c r="B46" s="26"/>
+      <c r="C46" s="26"/>
+      <c r="D46" s="26"/>
+      <c r="E46" s="26"/>
       <c r="F46">
         <f>SUM(C47:C55)</f>
         <v>2.75</v>
       </c>
       <c r="G46">
         <f>C47*D47+C50*D50+C52*D52+C54*D54</f>
-        <v>2.25</v>
+        <v>1.85</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -1384,7 +1382,7 @@
       <c r="D47" s="22">
         <v>1</v>
       </c>
-      <c r="E47" s="24"/>
+      <c r="E47" s="25"/>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="21"/>
@@ -1392,8 +1390,8 @@
         <v>44</v>
       </c>
       <c r="C48" s="21"/>
-      <c r="D48" s="33"/>
-      <c r="E48" s="33"/>
+      <c r="D48" s="23"/>
+      <c r="E48" s="23"/>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="21"/>
@@ -1401,8 +1399,8 @@
         <v>45</v>
       </c>
       <c r="C49" s="21"/>
-      <c r="D49" s="23"/>
-      <c r="E49" s="23"/>
+      <c r="D49" s="24"/>
+      <c r="E49" s="24"/>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="21">
@@ -1414,10 +1412,10 @@
       <c r="C50" s="21">
         <v>1</v>
       </c>
-      <c r="D50" s="27">
-        <v>0.5</v>
-      </c>
-      <c r="E50" s="24"/>
+      <c r="D50" s="32">
+        <v>0.1</v>
+      </c>
+      <c r="E50" s="25"/>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="21"/>
@@ -1425,8 +1423,8 @@
         <v>47</v>
       </c>
       <c r="C51" s="21"/>
-      <c r="D51" s="28"/>
-      <c r="E51" s="23"/>
+      <c r="D51" s="33"/>
+      <c r="E51" s="24"/>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="21">
@@ -1438,10 +1436,10 @@
       <c r="C52" s="21">
         <v>0.5</v>
       </c>
-      <c r="D52" s="27">
-        <v>1</v>
-      </c>
-      <c r="E52" s="24"/>
+      <c r="D52" s="32">
+        <v>1</v>
+      </c>
+      <c r="E52" s="25"/>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="21"/>
@@ -1449,8 +1447,8 @@
         <v>47</v>
       </c>
       <c r="C53" s="21"/>
-      <c r="D53" s="28"/>
-      <c r="E53" s="23"/>
+      <c r="D53" s="33"/>
+      <c r="E53" s="24"/>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="21">
@@ -1465,7 +1463,7 @@
       <c r="D54" s="22">
         <v>1</v>
       </c>
-      <c r="E54" s="24"/>
+      <c r="E54" s="25"/>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="21"/>
@@ -1473,22 +1471,45 @@
         <v>47</v>
       </c>
       <c r="C55" s="21"/>
-      <c r="D55" s="23"/>
-      <c r="E55" s="23"/>
+      <c r="D55" s="24"/>
+      <c r="E55" s="24"/>
     </row>
     <row r="57" spans="1:6">
       <c r="F57" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="D13:D16"/>
-    <mergeCell ref="E13:E16"/>
-    <mergeCell ref="A17:A22"/>
-    <mergeCell ref="C17:C22"/>
-    <mergeCell ref="D17:D22"/>
-    <mergeCell ref="E17:E22"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="E50:E51"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="A42:E42"/>
+    <mergeCell ref="A46:E46"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="E23:E25"/>
+    <mergeCell ref="E28:E31"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="C13:C16"/>
     <mergeCell ref="C47:C49"/>
     <mergeCell ref="D47:D49"/>
     <mergeCell ref="E47:E49"/>
@@ -1505,37 +1526,14 @@
     <mergeCell ref="D37:D40"/>
     <mergeCell ref="E37:E40"/>
     <mergeCell ref="A32:A33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="E23:E25"/>
-    <mergeCell ref="E28:E31"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="C13:C16"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="E50:E51"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="A42:E42"/>
-    <mergeCell ref="A46:E46"/>
-    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="D13:D16"/>
+    <mergeCell ref="E13:E16"/>
+    <mergeCell ref="A17:A22"/>
+    <mergeCell ref="C17:C22"/>
+    <mergeCell ref="D17:D22"/>
+    <mergeCell ref="E17:E22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>